<commit_message>
ultimos cambios: scanner global, estilos.
</commit_message>
<xml_diff>
--- a/back/istockBack/BackupMensual/backup_mensual_202508_ventas.xlsx
+++ b/back/istockBack/BackupMensual/backup_mensual_202508_ventas.xlsx
@@ -42,7 +42,7 @@
     <x:t>Equipo Parte de Pago</x:t>
   </x:si>
   <x:si>
-    <x:t>Goku</x:t>
+    <x:t>Nicolas Priotti</x:t>
   </x:si>
   <x:si>
     <x:t>Efectivo</x:t>
@@ -51,31 +51,43 @@
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>Vegeta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tarjeta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lucas</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">iPhone 11 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>sdfsf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>iPhone 14 Pro Max White - 90% - 128gb</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nico</x:t>
+    <x:t>Agustin Fossatto</x:t>
   </x:si>
   <x:si>
     <x:t>Transferencia</x:t>
   </x:si>
   <x:si>
-    <x:t>iPhone 15 Pro - Silver - 128gb - 93%</x:t>
+    <x:t>Nicolas Re</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diosito Kasoteira</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Otro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pedro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pablo Ramirez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Colapinto</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Lucas </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kevin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Prueba 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Prueba 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Juan</x:t>
   </x:si>
   <x:si>
     <x:t>Producto</x:t>
@@ -90,22 +102,34 @@
     <x:t>Ganancia</x:t>
   </x:si>
   <x:si>
-    <x:t>iPhone 15 Pro</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Macbook Pro 13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Macbook Air 13</x:t>
+    <x:t>Sin nombre</x:t>
   </x:si>
   <x:si>
     <x:t>Funda Trasparente</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">iPhone 16 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vidrio Templado</x:t>
+    <x:t>Funda Silicona</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Macbook Air</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barra Sonido Samsung</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Airpods</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Xiaomi s20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apple Watch 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PlayStation 5 Slim</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Macbook Pro</x:t>
   </x:si>
   <x:si>
     <x:t>Métrica</x:t>
@@ -172,20 +196,27 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -484,7 +515,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H6"/>
+  <x:dimension ref="A1:H13"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -518,25 +549,25 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0">
-        <x:v>1</x:v>
+        <x:v>3024</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C2" s="1">
-        <x:v>45874</x:v>
+        <x:v>45899</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0">
-        <x:v>2950</x:v>
+        <x:v>909.63</x:v>
       </x:c>
       <x:c r="F2" s="0">
-        <x:v>300</x:v>
+        <x:v>57.41</x:v>
       </x:c>
       <x:c r="G2" s="0">
-        <x:v>1315</x:v>
+        <x:v>1350</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
         <x:v>10</x:v>
@@ -544,25 +575,25 @@
     </x:row>
     <x:row r="3" spans="1:8">
       <x:c r="A3" s="0">
-        <x:v>2</x:v>
+        <x:v>3025</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="1">
-        <x:v>45874</x:v>
+        <x:v>45899</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="E3" s="0">
-        <x:v>14350</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="F3" s="0">
-        <x:v>1500</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="G3" s="0">
-        <x:v>1315</x:v>
+        <x:v>1370</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
         <x:v>10</x:v>
@@ -570,80 +601,262 @@
     </x:row>
     <x:row r="4" spans="1:8">
       <x:c r="A4" s="0">
-        <x:v>3</x:v>
+        <x:v>3026</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="C4" s="1">
-        <x:v>45875</x:v>
+        <x:v>45899</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="0">
-        <x:v>965</x:v>
+        <x:v>29.2</x:v>
       </x:c>
       <x:c r="F4" s="0">
-        <x:v>160</x:v>
+        <x:v>21.9</x:v>
       </x:c>
       <x:c r="G4" s="0">
-        <x:v>1315</x:v>
+        <x:v>1370</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
       <x:c r="A5" s="0">
-        <x:v>4</x:v>
+        <x:v>3027</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C5" s="1">
+        <x:v>45899</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C5" s="1">
-        <x:v>45875</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="E5" s="0">
-        <x:v>850</x:v>
+        <x:v>36.5</x:v>
       </x:c>
       <x:c r="F5" s="0">
-        <x:v>100</x:v>
+        <x:v>29.2</x:v>
       </x:c>
       <x:c r="G5" s="0">
-        <x:v>1310</x:v>
+        <x:v>1370</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="0">
-        <x:v>5</x:v>
+        <x:v>3028</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C6" s="1">
+        <x:v>45899</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="0">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="F6" s="0">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="G6" s="0">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" s="0">
+        <x:v>3029</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C6" s="1">
-        <x:v>45875</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="C7" s="1">
+        <x:v>45899</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E7" s="0">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="F7" s="0">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="G7" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" s="0">
+        <x:v>3030</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="E6" s="0">
-        <x:v>1875</x:v>
-      </x:c>
-      <x:c r="F6" s="0">
-        <x:v>265</x:v>
-      </x:c>
-      <x:c r="G6" s="0">
-        <x:v>1420</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
+      <x:c r="C8" s="1">
+        <x:v>45900</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="0">
+        <x:v>806.1</x:v>
+      </x:c>
+      <x:c r="F8" s="0">
+        <x:v>104.42</x:v>
+      </x:c>
+      <x:c r="G8" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" s="0">
+        <x:v>3031</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>19</x:v>
+      </x:c>
+      <x:c r="C9" s="1">
+        <x:v>45900</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E9" s="0">
+        <x:v>3000</x:v>
+      </x:c>
+      <x:c r="F9" s="0">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="G9" s="0">
+        <x:v>1200</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" s="0">
+        <x:v>3032</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C10" s="1">
+        <x:v>45900</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E10" s="0">
+        <x:v>155.84</x:v>
+      </x:c>
+      <x:c r="F10" s="0">
+        <x:v>54.38</x:v>
+      </x:c>
+      <x:c r="G10" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="0">
+        <x:v>3033</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C11" s="1">
+        <x:v>45900</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E11" s="0">
+        <x:v>244.6</x:v>
+      </x:c>
+      <x:c r="F11" s="0">
+        <x:v>41.68</x:v>
+      </x:c>
+      <x:c r="G11" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0">
+        <x:v>3034</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C12" s="1">
+        <x:v>45900</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E12" s="0">
+        <x:v>155.84</x:v>
+      </x:c>
+      <x:c r="F12" s="0">
+        <x:v>54.38</x:v>
+      </x:c>
+      <x:c r="G12" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="0">
+        <x:v>3035</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C13" s="2">
+        <x:v>45900.4570949074</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E13" s="0">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="F13" s="0">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="G13" s="0">
+        <x:v>1370</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -660,7 +873,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F12"/>
+  <x:dimension ref="A1:F24"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -671,239 +884,479 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="0">
-        <x:v>1</x:v>
+        <x:v>3024</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C2" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D2" s="0">
-        <x:v>850</x:v>
+        <x:v>900</x:v>
       </x:c>
       <x:c r="E2" s="0">
-        <x:v>850</x:v>
+        <x:v>900</x:v>
       </x:c>
       <x:c r="F2" s="0">
-        <x:v>100</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="0">
-        <x:v>1</x:v>
+        <x:v>3024</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C3" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D3" s="0">
-        <x:v>2100</x:v>
+        <x:v>3.7</x:v>
       </x:c>
       <x:c r="E3" s="0">
-        <x:v>2100</x:v>
+        <x:v>3.7</x:v>
       </x:c>
       <x:c r="F3" s="0">
-        <x:v>200</x:v>
+        <x:v>2.96</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="A4" s="0">
-        <x:v>2</x:v>
+        <x:v>3024</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C4" s="0">
-        <x:v>7</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D4" s="0">
-        <x:v>850</x:v>
+        <x:v>5.93</x:v>
       </x:c>
       <x:c r="E4" s="0">
-        <x:v>5950</x:v>
+        <x:v>5.93</x:v>
       </x:c>
       <x:c r="F4" s="0">
-        <x:v>700</x:v>
+        <x:v>4.45</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0">
-        <x:v>2</x:v>
+        <x:v>3025</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C5" s="0">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D5" s="0">
-        <x:v>2100</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="E5" s="0">
-        <x:v>8400</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="F5" s="0">
-        <x:v>800</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0">
-        <x:v>3</x:v>
+        <x:v>3026</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C6" s="0">
-        <x:v>1</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D6" s="0">
-        <x:v>950</x:v>
+        <x:v>5.84</x:v>
       </x:c>
       <x:c r="E6" s="0">
-        <x:v>950</x:v>
+        <x:v>29.2</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>150</x:v>
+        <x:v>21.9</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="A7" s="0">
-        <x:v>3</x:v>
+        <x:v>3027</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C7" s="0">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D7" s="0">
-        <x:v>15</x:v>
+        <x:v>3.65</x:v>
       </x:c>
       <x:c r="E7" s="0">
-        <x:v>15</x:v>
+        <x:v>36.5</x:v>
       </x:c>
       <x:c r="F7" s="0">
-        <x:v>10</x:v>
+        <x:v>29.2</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="0">
-        <x:v>4</x:v>
+        <x:v>3028</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C8" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D8" s="0">
-        <x:v>850</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="E8" s="0">
-        <x:v>850</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F8" s="0">
-        <x:v>100</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="0">
-        <x:v>5</x:v>
+        <x:v>3029</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C9" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D9" s="0">
-        <x:v>900</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="E9" s="0">
-        <x:v>900</x:v>
+        <x:v>850</x:v>
       </x:c>
       <x:c r="F9" s="0">
-        <x:v>100</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="0">
-        <x:v>5</x:v>
+        <x:v>3029</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C10" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D10" s="0">
-        <x:v>15</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="E10" s="0">
-        <x:v>15</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F10" s="0">
-        <x:v>10</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="0">
-        <x:v>5</x:v>
+        <x:v>3030</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C11" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D11" s="0">
-        <x:v>10</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="E11" s="0">
-        <x:v>10</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F11" s="0">
-        <x:v>5</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="0">
-        <x:v>5</x:v>
+        <x:v>3030</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C12" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D12" s="0">
-        <x:v>950</x:v>
+        <x:v>0.26</x:v>
       </x:c>
       <x:c r="E12" s="0">
-        <x:v>950</x:v>
+        <x:v>0.26</x:v>
       </x:c>
       <x:c r="F12" s="0">
+        <x:v>0.04</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0">
+        <x:v>3030</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C13" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D13" s="0">
+        <x:v>550</x:v>
+      </x:c>
+      <x:c r="E13" s="0">
+        <x:v>550</x:v>
+      </x:c>
+      <x:c r="F13" s="0">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0">
+        <x:v>3030</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C14" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D14" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="E14" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="F14" s="0">
+        <x:v>4.38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0">
+        <x:v>3031</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C15" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D15" s="0">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="E15" s="0">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="F15" s="0">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0">
+        <x:v>3031</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C16" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D16" s="0">
+        <x:v>650</x:v>
+      </x:c>
+      <x:c r="E16" s="0">
+        <x:v>650</x:v>
+      </x:c>
+      <x:c r="F16" s="0">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0">
+        <x:v>3031</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C17" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D17" s="0">
+        <x:v>2000</x:v>
+      </x:c>
+      <x:c r="E17" s="0">
+        <x:v>2000</x:v>
+      </x:c>
+      <x:c r="F17" s="0">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0">
+        <x:v>3032</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C18" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D18" s="0">
         <x:v>150</x:v>
+      </x:c>
+      <x:c r="E18" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="F18" s="0">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0">
+        <x:v>3032</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C19" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D19" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="E19" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="F19" s="0">
+        <x:v>4.38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0">
+        <x:v>3033</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C20" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D20" s="0">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="E20" s="0">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="F20" s="0">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0">
+        <x:v>3033</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C21" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D21" s="0">
+        <x:v>3.65</x:v>
+      </x:c>
+      <x:c r="E21" s="0">
+        <x:v>14.6</x:v>
+      </x:c>
+      <x:c r="F21" s="0">
+        <x:v>11.68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0">
+        <x:v>3034</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C22" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D22" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="E22" s="0">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="F22" s="0">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0">
+        <x:v>3034</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C23" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D23" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="E23" s="0">
+        <x:v>5.84</x:v>
+      </x:c>
+      <x:c r="F23" s="0">
+        <x:v>4.38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0">
+        <x:v>3035</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C24" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D24" s="0">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="E24" s="0">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="F24" s="0">
+        <x:v>50</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -928,50 +1381,50 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B2" s="0">
-        <x:v>3084700</x:v>
+        <x:v>1080668.7</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
       <x:c r="A3" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B3" s="0">
-        <x:v>2325</x:v>
+        <x:v>813.37</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
       <x:c r="A4" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B4" s="0">
-        <x:v>350</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
       <x:c r="A5" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B5" s="0">
-        <x:v>1975</x:v>
+        <x:v>593.37</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
       <x:c r="A6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B6" s="0">
-        <x:v>2636625</x:v>
+        <x:v>805005.3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>